<commit_message>
All Mobile TC execution
</commit_message>
<xml_diff>
--- a/testData/SFI_AllMobile_Tbl_RThree.xlsx
+++ b/testData/SFI_AllMobile_Tbl_RThree.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="125">
   <si>
     <t>BuildUrl</t>
   </si>
@@ -379,6 +379,21 @@
   </si>
   <si>
     <t>formshow_15112023</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:00 AM to 09:04 AM ]</t>
+  </si>
+  <si>
+    <t>16/11/2023</t>
+  </si>
+  <si>
+    <t>voice_record_16112023</t>
+  </si>
+  <si>
+    <t>formshow_16112023</t>
+  </si>
+  <si>
+    <t>Appointment Date : 16/11/2023, Time : [ 09:05 AM to 09:09 AM ]</t>
   </si>
 </sst>
 </file>
@@ -958,7 +973,7 @@
         <v>50</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="O2" t="s" s="0">
         <v>51</v>
@@ -1000,7 +1015,7 @@
         <v>56</v>
       </c>
       <c r="AB2" t="s" s="0">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="AC2" t="s" s="0">
         <v>58</v>
@@ -1045,7 +1060,7 @@
         <v>61</v>
       </c>
       <c r="AR2" t="s" s="0">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="AS2" t="s" s="0">
         <v>57</v>
@@ -1054,7 +1069,7 @@
         <v>65</v>
       </c>
       <c r="AU2" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="AV2" s="3" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
run sfi and check
</commit_message>
<xml_diff>
--- a/testData/SFI_AllMobile_Tbl_RThree.xlsx
+++ b/testData/SFI_AllMobile_Tbl_RThree.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="136">
   <si>
     <t>BuildUrl</t>
   </si>
@@ -418,6 +418,15 @@
   </si>
   <si>
     <t>Appointment Date : 21/11/2023, Time : [ 09:10 AM to 09:14 AM ]</t>
+  </si>
+  <si>
+    <t>Appointment Date : 22/11/2023, Time : [ 09:05 AM to 09:09 AM ]</t>
+  </si>
+  <si>
+    <t>22/11/2023</t>
+  </si>
+  <si>
+    <t>Appointment Date : 22/11/2023, Time : [ 09:10 AM to 09:14 AM ]</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1006,7 @@
         <v>50</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="O2" t="s" s="0">
         <v>51</v>
@@ -1039,7 +1048,7 @@
         <v>56</v>
       </c>
       <c r="AB2" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AC2" t="s" s="0">
         <v>58</v>

</xml_diff>